<commit_message>
feat: add options, logo parts to confirmation
</commit_message>
<xml_diff>
--- a/server/orders/OrderConfirmationTmpRu.xlsx
+++ b/server/orders/OrderConfirmationTmpRu.xlsx
@@ -2037,7 +2037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="347">
+  <cellXfs count="345">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
@@ -2891,38 +2891,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3080,6 +3048,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3509,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,21 +5449,21 @@
       <c r="AE42" s="84"/>
     </row>
     <row r="43" spans="1:31" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="314" t="s">
+      <c r="A43" s="306" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="315"/>
-      <c r="C43" s="315"/>
-      <c r="D43" s="315"/>
-      <c r="E43" s="315"/>
-      <c r="F43" s="315"/>
-      <c r="G43" s="315"/>
-      <c r="H43" s="315"/>
-      <c r="I43" s="315"/>
-      <c r="J43" s="315"/>
-      <c r="K43" s="315"/>
-      <c r="L43" s="315"/>
-      <c r="M43" s="316"/>
+      <c r="B43" s="307"/>
+      <c r="C43" s="307"/>
+      <c r="D43" s="307"/>
+      <c r="E43" s="307"/>
+      <c r="F43" s="307"/>
+      <c r="G43" s="307"/>
+      <c r="H43" s="307"/>
+      <c r="I43" s="307"/>
+      <c r="J43" s="307"/>
+      <c r="K43" s="307"/>
+      <c r="L43" s="307"/>
+      <c r="M43" s="308"/>
       <c r="N43" s="289" t="s">
         <v>118</v>
       </c>
@@ -5500,19 +5492,19 @@
       <c r="AE43" s="84"/>
     </row>
     <row r="44" spans="1:31" s="71" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="291"/>
-      <c r="B44" s="170"/>
-      <c r="C44" s="170"/>
-      <c r="D44" s="170"/>
-      <c r="E44" s="170"/>
-      <c r="F44" s="170"/>
-      <c r="G44" s="170"/>
-      <c r="H44" s="170"/>
-      <c r="I44" s="170"/>
-      <c r="J44" s="170"/>
-      <c r="K44" s="170"/>
-      <c r="L44" s="170"/>
-      <c r="M44" s="292"/>
+      <c r="A44" s="339"/>
+      <c r="B44" s="340"/>
+      <c r="C44" s="340"/>
+      <c r="D44" s="340"/>
+      <c r="E44" s="340"/>
+      <c r="F44" s="340"/>
+      <c r="G44" s="340"/>
+      <c r="H44" s="340"/>
+      <c r="I44" s="340"/>
+      <c r="J44" s="340"/>
+      <c r="K44" s="340"/>
+      <c r="L44" s="340"/>
+      <c r="M44" s="341"/>
       <c r="N44" s="274" t="s">
         <v>120</v>
       </c>
@@ -5541,19 +5533,19 @@
       <c r="AE44" s="84"/>
     </row>
     <row r="45" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="293"/>
-      <c r="B45" s="294"/>
-      <c r="C45" s="294"/>
-      <c r="D45" s="294"/>
-      <c r="E45" s="294"/>
-      <c r="F45" s="294"/>
-      <c r="G45" s="294"/>
-      <c r="H45" s="294"/>
-      <c r="I45" s="294"/>
-      <c r="J45" s="294"/>
-      <c r="K45" s="294"/>
-      <c r="L45" s="294"/>
-      <c r="M45" s="295"/>
+      <c r="A45" s="294"/>
+      <c r="B45" s="295"/>
+      <c r="C45" s="295"/>
+      <c r="D45" s="295"/>
+      <c r="E45" s="295"/>
+      <c r="F45" s="295"/>
+      <c r="G45" s="295"/>
+      <c r="H45" s="295"/>
+      <c r="I45" s="295"/>
+      <c r="J45" s="295"/>
+      <c r="K45" s="295"/>
+      <c r="L45" s="295"/>
+      <c r="M45" s="296"/>
       <c r="N45" s="190" t="s">
         <v>124</v>
       </c>
@@ -5584,19 +5576,19 @@
       <c r="AE45" s="84"/>
     </row>
     <row r="46" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="293"/>
-      <c r="B46" s="294"/>
-      <c r="C46" s="294"/>
-      <c r="D46" s="294"/>
-      <c r="E46" s="294"/>
-      <c r="F46" s="294"/>
-      <c r="G46" s="294"/>
-      <c r="H46" s="294"/>
-      <c r="I46" s="294"/>
-      <c r="J46" s="294"/>
-      <c r="K46" s="294"/>
-      <c r="L46" s="294"/>
-      <c r="M46" s="295"/>
+      <c r="A46" s="294"/>
+      <c r="B46" s="295"/>
+      <c r="C46" s="295"/>
+      <c r="D46" s="295"/>
+      <c r="E46" s="295"/>
+      <c r="F46" s="295"/>
+      <c r="G46" s="295"/>
+      <c r="H46" s="295"/>
+      <c r="I46" s="295"/>
+      <c r="J46" s="295"/>
+      <c r="K46" s="295"/>
+      <c r="L46" s="295"/>
+      <c r="M46" s="296"/>
       <c r="N46" s="190" t="s">
         <v>125</v>
       </c>
@@ -5625,19 +5617,19 @@
       <c r="AE46" s="84"/>
     </row>
     <row r="47" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="293"/>
-      <c r="B47" s="294"/>
-      <c r="C47" s="294"/>
-      <c r="D47" s="294"/>
-      <c r="E47" s="294"/>
-      <c r="F47" s="294"/>
-      <c r="G47" s="294"/>
-      <c r="H47" s="294"/>
-      <c r="I47" s="294"/>
-      <c r="J47" s="294"/>
-      <c r="K47" s="294"/>
-      <c r="L47" s="294"/>
-      <c r="M47" s="295"/>
+      <c r="A47" s="294"/>
+      <c r="B47" s="295"/>
+      <c r="C47" s="295"/>
+      <c r="D47" s="295"/>
+      <c r="E47" s="295"/>
+      <c r="F47" s="295"/>
+      <c r="G47" s="295"/>
+      <c r="H47" s="295"/>
+      <c r="I47" s="295"/>
+      <c r="J47" s="295"/>
+      <c r="K47" s="295"/>
+      <c r="L47" s="295"/>
+      <c r="M47" s="296"/>
       <c r="N47" s="190" t="s">
         <v>126</v>
       </c>
@@ -5666,19 +5658,19 @@
       <c r="AE47" s="84"/>
     </row>
     <row r="48" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="296"/>
-      <c r="B48" s="297"/>
-      <c r="C48" s="297"/>
-      <c r="D48" s="297"/>
-      <c r="E48" s="297"/>
-      <c r="F48" s="297"/>
-      <c r="G48" s="297"/>
-      <c r="H48" s="297"/>
-      <c r="I48" s="297"/>
-      <c r="J48" s="297"/>
-      <c r="K48" s="297"/>
-      <c r="L48" s="297"/>
-      <c r="M48" s="298"/>
+      <c r="A48" s="342"/>
+      <c r="B48" s="343"/>
+      <c r="C48" s="343"/>
+      <c r="D48" s="343"/>
+      <c r="E48" s="343"/>
+      <c r="F48" s="343"/>
+      <c r="G48" s="343"/>
+      <c r="H48" s="343"/>
+      <c r="I48" s="343"/>
+      <c r="J48" s="343"/>
+      <c r="K48" s="343"/>
+      <c r="L48" s="343"/>
+      <c r="M48" s="344"/>
       <c r="N48" s="239" t="s">
         <v>127</v>
       </c>
@@ -5707,34 +5699,34 @@
       <c r="AE48" s="84"/>
     </row>
     <row r="49" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="299" t="s">
+      <c r="A49" s="291" t="s">
         <v>128</v>
       </c>
-      <c r="B49" s="300"/>
-      <c r="C49" s="300"/>
-      <c r="D49" s="300"/>
-      <c r="E49" s="300"/>
-      <c r="F49" s="300"/>
-      <c r="G49" s="300"/>
-      <c r="H49" s="300"/>
-      <c r="I49" s="300"/>
-      <c r="J49" s="300"/>
-      <c r="K49" s="300"/>
-      <c r="L49" s="300"/>
-      <c r="M49" s="300"/>
-      <c r="N49" s="300"/>
-      <c r="O49" s="300"/>
-      <c r="P49" s="300"/>
-      <c r="Q49" s="300"/>
-      <c r="R49" s="300"/>
-      <c r="S49" s="300"/>
-      <c r="T49" s="300"/>
-      <c r="U49" s="300"/>
-      <c r="V49" s="300"/>
-      <c r="W49" s="300"/>
-      <c r="X49" s="300"/>
-      <c r="Y49" s="300"/>
-      <c r="Z49" s="301"/>
+      <c r="B49" s="292"/>
+      <c r="C49" s="292"/>
+      <c r="D49" s="292"/>
+      <c r="E49" s="292"/>
+      <c r="F49" s="292"/>
+      <c r="G49" s="292"/>
+      <c r="H49" s="292"/>
+      <c r="I49" s="292"/>
+      <c r="J49" s="292"/>
+      <c r="K49" s="292"/>
+      <c r="L49" s="292"/>
+      <c r="M49" s="292"/>
+      <c r="N49" s="292"/>
+      <c r="O49" s="292"/>
+      <c r="P49" s="292"/>
+      <c r="Q49" s="292"/>
+      <c r="R49" s="292"/>
+      <c r="S49" s="292"/>
+      <c r="T49" s="292"/>
+      <c r="U49" s="292"/>
+      <c r="V49" s="292"/>
+      <c r="W49" s="292"/>
+      <c r="X49" s="292"/>
+      <c r="Y49" s="292"/>
+      <c r="Z49" s="293"/>
       <c r="AA49" s="82"/>
       <c r="AB49" s="4" t="str">
         <f>PriceList!F47</f>
@@ -5748,32 +5740,32 @@
       <c r="AE49" s="84"/>
     </row>
     <row r="50" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="302"/>
-      <c r="B50" s="303"/>
-      <c r="C50" s="303"/>
-      <c r="D50" s="303"/>
-      <c r="E50" s="303"/>
-      <c r="F50" s="303"/>
-      <c r="G50" s="303"/>
-      <c r="H50" s="303"/>
-      <c r="I50" s="303"/>
-      <c r="J50" s="303"/>
-      <c r="K50" s="303"/>
-      <c r="L50" s="303"/>
-      <c r="M50" s="303"/>
-      <c r="N50" s="303"/>
-      <c r="O50" s="303"/>
-      <c r="P50" s="303"/>
-      <c r="Q50" s="303"/>
-      <c r="R50" s="303"/>
-      <c r="S50" s="303"/>
-      <c r="T50" s="303"/>
-      <c r="U50" s="303"/>
-      <c r="V50" s="303"/>
-      <c r="W50" s="303"/>
-      <c r="X50" s="303"/>
-      <c r="Y50" s="303"/>
-      <c r="Z50" s="304"/>
+      <c r="A50" s="294"/>
+      <c r="B50" s="295"/>
+      <c r="C50" s="295"/>
+      <c r="D50" s="295"/>
+      <c r="E50" s="295"/>
+      <c r="F50" s="295"/>
+      <c r="G50" s="295"/>
+      <c r="H50" s="295"/>
+      <c r="I50" s="295"/>
+      <c r="J50" s="295"/>
+      <c r="K50" s="295"/>
+      <c r="L50" s="295"/>
+      <c r="M50" s="295"/>
+      <c r="N50" s="295"/>
+      <c r="O50" s="295"/>
+      <c r="P50" s="295"/>
+      <c r="Q50" s="295"/>
+      <c r="R50" s="295"/>
+      <c r="S50" s="295"/>
+      <c r="T50" s="295"/>
+      <c r="U50" s="295"/>
+      <c r="V50" s="295"/>
+      <c r="W50" s="295"/>
+      <c r="X50" s="295"/>
+      <c r="Y50" s="295"/>
+      <c r="Z50" s="296"/>
       <c r="AA50" s="82"/>
       <c r="AB50" s="4" t="str">
         <f>PriceList!F48</f>
@@ -5787,32 +5779,32 @@
       <c r="AE50" s="84"/>
     </row>
     <row r="51" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="302"/>
-      <c r="B51" s="303"/>
-      <c r="C51" s="303"/>
-      <c r="D51" s="303"/>
-      <c r="E51" s="303"/>
-      <c r="F51" s="303"/>
-      <c r="G51" s="303"/>
-      <c r="H51" s="303"/>
-      <c r="I51" s="303"/>
-      <c r="J51" s="303"/>
-      <c r="K51" s="303"/>
-      <c r="L51" s="303"/>
-      <c r="M51" s="303"/>
-      <c r="N51" s="303"/>
-      <c r="O51" s="303"/>
-      <c r="P51" s="303"/>
-      <c r="Q51" s="303"/>
-      <c r="R51" s="303"/>
-      <c r="S51" s="303"/>
-      <c r="T51" s="303"/>
-      <c r="U51" s="303"/>
-      <c r="V51" s="303"/>
-      <c r="W51" s="303"/>
-      <c r="X51" s="303"/>
-      <c r="Y51" s="303"/>
-      <c r="Z51" s="304"/>
+      <c r="A51" s="294"/>
+      <c r="B51" s="295"/>
+      <c r="C51" s="295"/>
+      <c r="D51" s="295"/>
+      <c r="E51" s="295"/>
+      <c r="F51" s="295"/>
+      <c r="G51" s="295"/>
+      <c r="H51" s="295"/>
+      <c r="I51" s="295"/>
+      <c r="J51" s="295"/>
+      <c r="K51" s="295"/>
+      <c r="L51" s="295"/>
+      <c r="M51" s="295"/>
+      <c r="N51" s="295"/>
+      <c r="O51" s="295"/>
+      <c r="P51" s="295"/>
+      <c r="Q51" s="295"/>
+      <c r="R51" s="295"/>
+      <c r="S51" s="295"/>
+      <c r="T51" s="295"/>
+      <c r="U51" s="295"/>
+      <c r="V51" s="295"/>
+      <c r="W51" s="295"/>
+      <c r="X51" s="295"/>
+      <c r="Y51" s="295"/>
+      <c r="Z51" s="296"/>
       <c r="AA51" s="82"/>
       <c r="AB51" s="4" t="str">
         <f>PriceList!F49</f>
@@ -5826,32 +5818,32 @@
       <c r="AE51" s="84"/>
     </row>
     <row r="52" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="302"/>
-      <c r="B52" s="303"/>
-      <c r="C52" s="303"/>
-      <c r="D52" s="303"/>
-      <c r="E52" s="303"/>
-      <c r="F52" s="303"/>
-      <c r="G52" s="303"/>
-      <c r="H52" s="303"/>
-      <c r="I52" s="303"/>
-      <c r="J52" s="303"/>
-      <c r="K52" s="303"/>
-      <c r="L52" s="303"/>
-      <c r="M52" s="303"/>
-      <c r="N52" s="303"/>
-      <c r="O52" s="303"/>
-      <c r="P52" s="303"/>
-      <c r="Q52" s="303"/>
-      <c r="R52" s="303"/>
-      <c r="S52" s="303"/>
-      <c r="T52" s="303"/>
-      <c r="U52" s="303"/>
-      <c r="V52" s="303"/>
-      <c r="W52" s="303"/>
-      <c r="X52" s="303"/>
-      <c r="Y52" s="303"/>
-      <c r="Z52" s="304"/>
+      <c r="A52" s="294"/>
+      <c r="B52" s="295"/>
+      <c r="C52" s="295"/>
+      <c r="D52" s="295"/>
+      <c r="E52" s="295"/>
+      <c r="F52" s="295"/>
+      <c r="G52" s="295"/>
+      <c r="H52" s="295"/>
+      <c r="I52" s="295"/>
+      <c r="J52" s="295"/>
+      <c r="K52" s="295"/>
+      <c r="L52" s="295"/>
+      <c r="M52" s="295"/>
+      <c r="N52" s="295"/>
+      <c r="O52" s="295"/>
+      <c r="P52" s="295"/>
+      <c r="Q52" s="295"/>
+      <c r="R52" s="295"/>
+      <c r="S52" s="295"/>
+      <c r="T52" s="295"/>
+      <c r="U52" s="295"/>
+      <c r="V52" s="295"/>
+      <c r="W52" s="295"/>
+      <c r="X52" s="295"/>
+      <c r="Y52" s="295"/>
+      <c r="Z52" s="296"/>
       <c r="AA52" s="82"/>
       <c r="AB52" s="4" t="str">
         <f>PriceList!F50</f>
@@ -5865,32 +5857,32 @@
       <c r="AE52" s="84"/>
     </row>
     <row r="53" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="302"/>
-      <c r="B53" s="303"/>
-      <c r="C53" s="303"/>
-      <c r="D53" s="303"/>
-      <c r="E53" s="303"/>
-      <c r="F53" s="303"/>
-      <c r="G53" s="303"/>
-      <c r="H53" s="303"/>
-      <c r="I53" s="303"/>
-      <c r="J53" s="303"/>
-      <c r="K53" s="303"/>
-      <c r="L53" s="303"/>
-      <c r="M53" s="303"/>
-      <c r="N53" s="303"/>
-      <c r="O53" s="303"/>
-      <c r="P53" s="303"/>
-      <c r="Q53" s="303"/>
-      <c r="R53" s="303"/>
-      <c r="S53" s="303"/>
-      <c r="T53" s="303"/>
-      <c r="U53" s="303"/>
-      <c r="V53" s="303"/>
-      <c r="W53" s="303"/>
-      <c r="X53" s="303"/>
-      <c r="Y53" s="303"/>
-      <c r="Z53" s="304"/>
+      <c r="A53" s="294"/>
+      <c r="B53" s="295"/>
+      <c r="C53" s="295"/>
+      <c r="D53" s="295"/>
+      <c r="E53" s="295"/>
+      <c r="F53" s="295"/>
+      <c r="G53" s="295"/>
+      <c r="H53" s="295"/>
+      <c r="I53" s="295"/>
+      <c r="J53" s="295"/>
+      <c r="K53" s="295"/>
+      <c r="L53" s="295"/>
+      <c r="M53" s="295"/>
+      <c r="N53" s="295"/>
+      <c r="O53" s="295"/>
+      <c r="P53" s="295"/>
+      <c r="Q53" s="295"/>
+      <c r="R53" s="295"/>
+      <c r="S53" s="295"/>
+      <c r="T53" s="295"/>
+      <c r="U53" s="295"/>
+      <c r="V53" s="295"/>
+      <c r="W53" s="295"/>
+      <c r="X53" s="295"/>
+      <c r="Y53" s="295"/>
+      <c r="Z53" s="296"/>
       <c r="AA53" s="82"/>
       <c r="AB53" s="4" t="str">
         <f>PriceList!F51</f>
@@ -5904,32 +5896,32 @@
       <c r="AE53" s="84"/>
     </row>
     <row r="54" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="302"/>
-      <c r="B54" s="303"/>
-      <c r="C54" s="303"/>
-      <c r="D54" s="303"/>
-      <c r="E54" s="303"/>
-      <c r="F54" s="303"/>
-      <c r="G54" s="303"/>
-      <c r="H54" s="303"/>
-      <c r="I54" s="303"/>
-      <c r="J54" s="303"/>
-      <c r="K54" s="303"/>
-      <c r="L54" s="303"/>
-      <c r="M54" s="303"/>
-      <c r="N54" s="303"/>
-      <c r="O54" s="303"/>
-      <c r="P54" s="303"/>
-      <c r="Q54" s="303"/>
-      <c r="R54" s="303"/>
-      <c r="S54" s="303"/>
-      <c r="T54" s="303"/>
-      <c r="U54" s="303"/>
-      <c r="V54" s="303"/>
-      <c r="W54" s="303"/>
-      <c r="X54" s="303"/>
-      <c r="Y54" s="303"/>
-      <c r="Z54" s="304"/>
+      <c r="A54" s="294"/>
+      <c r="B54" s="295"/>
+      <c r="C54" s="295"/>
+      <c r="D54" s="295"/>
+      <c r="E54" s="295"/>
+      <c r="F54" s="295"/>
+      <c r="G54" s="295"/>
+      <c r="H54" s="295"/>
+      <c r="I54" s="295"/>
+      <c r="J54" s="295"/>
+      <c r="K54" s="295"/>
+      <c r="L54" s="295"/>
+      <c r="M54" s="295"/>
+      <c r="N54" s="295"/>
+      <c r="O54" s="295"/>
+      <c r="P54" s="295"/>
+      <c r="Q54" s="295"/>
+      <c r="R54" s="295"/>
+      <c r="S54" s="295"/>
+      <c r="T54" s="295"/>
+      <c r="U54" s="295"/>
+      <c r="V54" s="295"/>
+      <c r="W54" s="295"/>
+      <c r="X54" s="295"/>
+      <c r="Y54" s="295"/>
+      <c r="Z54" s="296"/>
       <c r="AA54" s="82"/>
       <c r="AB54" s="4" t="str">
         <f>PriceList!F52</f>
@@ -5943,34 +5935,34 @@
       <c r="AE54" s="84"/>
     </row>
     <row r="55" spans="1:31" s="71" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="305" t="s">
+      <c r="A55" s="297" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="306"/>
-      <c r="C55" s="306"/>
-      <c r="D55" s="306"/>
-      <c r="E55" s="306"/>
-      <c r="F55" s="306"/>
-      <c r="G55" s="306"/>
-      <c r="H55" s="306"/>
-      <c r="I55" s="306"/>
-      <c r="J55" s="306"/>
-      <c r="K55" s="306"/>
-      <c r="L55" s="306"/>
-      <c r="M55" s="306"/>
-      <c r="N55" s="306"/>
-      <c r="O55" s="306"/>
-      <c r="P55" s="306"/>
-      <c r="Q55" s="306"/>
-      <c r="R55" s="306"/>
-      <c r="S55" s="306"/>
-      <c r="T55" s="306"/>
-      <c r="U55" s="306"/>
-      <c r="V55" s="306"/>
-      <c r="W55" s="306"/>
-      <c r="X55" s="306"/>
-      <c r="Y55" s="306"/>
-      <c r="Z55" s="307"/>
+      <c r="B55" s="298"/>
+      <c r="C55" s="298"/>
+      <c r="D55" s="298"/>
+      <c r="E55" s="298"/>
+      <c r="F55" s="298"/>
+      <c r="G55" s="298"/>
+      <c r="H55" s="298"/>
+      <c r="I55" s="298"/>
+      <c r="J55" s="298"/>
+      <c r="K55" s="298"/>
+      <c r="L55" s="298"/>
+      <c r="M55" s="298"/>
+      <c r="N55" s="298"/>
+      <c r="O55" s="298"/>
+      <c r="P55" s="298"/>
+      <c r="Q55" s="298"/>
+      <c r="R55" s="298"/>
+      <c r="S55" s="298"/>
+      <c r="T55" s="298"/>
+      <c r="U55" s="298"/>
+      <c r="V55" s="298"/>
+      <c r="W55" s="298"/>
+      <c r="X55" s="298"/>
+      <c r="Y55" s="298"/>
+      <c r="Z55" s="299"/>
       <c r="AA55" s="82"/>
       <c r="AB55" s="4" t="str">
         <f>PriceList!F53</f>
@@ -5984,36 +5976,36 @@
       <c r="AE55" s="84"/>
     </row>
     <row r="56" spans="1:31" s="71" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="308" t="s">
+      <c r="A56" s="300" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="309"/>
-      <c r="C56" s="309"/>
-      <c r="D56" s="309"/>
-      <c r="E56" s="309"/>
-      <c r="F56" s="309"/>
-      <c r="G56" s="310"/>
-      <c r="H56" s="311"/>
-      <c r="I56" s="312"/>
-      <c r="J56" s="313"/>
-      <c r="K56" s="319"/>
-      <c r="L56" s="320"/>
-      <c r="M56" s="321"/>
-      <c r="N56" s="318" t="s">
+      <c r="B56" s="301"/>
+      <c r="C56" s="301"/>
+      <c r="D56" s="301"/>
+      <c r="E56" s="301"/>
+      <c r="F56" s="301"/>
+      <c r="G56" s="302"/>
+      <c r="H56" s="303"/>
+      <c r="I56" s="304"/>
+      <c r="J56" s="305"/>
+      <c r="K56" s="311"/>
+      <c r="L56" s="312"/>
+      <c r="M56" s="313"/>
+      <c r="N56" s="310" t="s">
         <v>131</v>
       </c>
-      <c r="O56" s="309"/>
-      <c r="P56" s="309"/>
-      <c r="Q56" s="309"/>
-      <c r="R56" s="309"/>
-      <c r="S56" s="309"/>
-      <c r="T56" s="310"/>
-      <c r="U56" s="311"/>
-      <c r="V56" s="312"/>
-      <c r="W56" s="313"/>
-      <c r="X56" s="311"/>
-      <c r="Y56" s="312"/>
-      <c r="Z56" s="317"/>
+      <c r="O56" s="301"/>
+      <c r="P56" s="301"/>
+      <c r="Q56" s="301"/>
+      <c r="R56" s="301"/>
+      <c r="S56" s="301"/>
+      <c r="T56" s="302"/>
+      <c r="U56" s="303"/>
+      <c r="V56" s="304"/>
+      <c r="W56" s="305"/>
+      <c r="X56" s="303"/>
+      <c r="Y56" s="304"/>
+      <c r="Z56" s="309"/>
       <c r="AA56" s="82"/>
       <c r="AB56" s="4" t="str">
         <f>PriceList!F54</f>
@@ -6027,36 +6019,36 @@
       <c r="AE56" s="84"/>
     </row>
     <row r="57" spans="1:31" s="71" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="308" t="s">
+      <c r="A57" s="300" t="s">
         <v>201</v>
       </c>
-      <c r="B57" s="309"/>
-      <c r="C57" s="309"/>
-      <c r="D57" s="309"/>
-      <c r="E57" s="309"/>
-      <c r="F57" s="309"/>
-      <c r="G57" s="310"/>
-      <c r="H57" s="311"/>
-      <c r="I57" s="312"/>
-      <c r="J57" s="313"/>
-      <c r="K57" s="322"/>
-      <c r="L57" s="323"/>
-      <c r="M57" s="324"/>
-      <c r="N57" s="318" t="s">
+      <c r="B57" s="301"/>
+      <c r="C57" s="301"/>
+      <c r="D57" s="301"/>
+      <c r="E57" s="301"/>
+      <c r="F57" s="301"/>
+      <c r="G57" s="302"/>
+      <c r="H57" s="303"/>
+      <c r="I57" s="304"/>
+      <c r="J57" s="305"/>
+      <c r="K57" s="314"/>
+      <c r="L57" s="315"/>
+      <c r="M57" s="316"/>
+      <c r="N57" s="310" t="s">
         <v>203</v>
       </c>
-      <c r="O57" s="309"/>
-      <c r="P57" s="309"/>
-      <c r="Q57" s="309"/>
-      <c r="R57" s="309"/>
-      <c r="S57" s="309"/>
-      <c r="T57" s="310"/>
-      <c r="U57" s="311"/>
-      <c r="V57" s="312"/>
-      <c r="W57" s="313"/>
-      <c r="X57" s="311"/>
-      <c r="Y57" s="312"/>
-      <c r="Z57" s="317"/>
+      <c r="O57" s="301"/>
+      <c r="P57" s="301"/>
+      <c r="Q57" s="301"/>
+      <c r="R57" s="301"/>
+      <c r="S57" s="301"/>
+      <c r="T57" s="302"/>
+      <c r="U57" s="303"/>
+      <c r="V57" s="304"/>
+      <c r="W57" s="305"/>
+      <c r="X57" s="303"/>
+      <c r="Y57" s="304"/>
+      <c r="Z57" s="309"/>
       <c r="AA57" s="82"/>
       <c r="AB57" s="4" t="str">
         <f>PriceList!F55</f>
@@ -6070,36 +6062,36 @@
       <c r="AE57" s="84"/>
     </row>
     <row r="58" spans="1:31" s="71" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="308" t="s">
+      <c r="A58" s="300" t="s">
         <v>202</v>
       </c>
-      <c r="B58" s="309"/>
-      <c r="C58" s="309"/>
-      <c r="D58" s="309"/>
-      <c r="E58" s="309"/>
-      <c r="F58" s="309"/>
-      <c r="G58" s="310"/>
-      <c r="H58" s="311"/>
-      <c r="I58" s="312"/>
-      <c r="J58" s="313"/>
-      <c r="K58" s="322"/>
-      <c r="L58" s="323"/>
-      <c r="M58" s="324"/>
-      <c r="N58" s="318" t="s">
+      <c r="B58" s="301"/>
+      <c r="C58" s="301"/>
+      <c r="D58" s="301"/>
+      <c r="E58" s="301"/>
+      <c r="F58" s="301"/>
+      <c r="G58" s="302"/>
+      <c r="H58" s="303"/>
+      <c r="I58" s="304"/>
+      <c r="J58" s="305"/>
+      <c r="K58" s="314"/>
+      <c r="L58" s="315"/>
+      <c r="M58" s="316"/>
+      <c r="N58" s="310" t="s">
         <v>132</v>
       </c>
-      <c r="O58" s="309"/>
-      <c r="P58" s="309"/>
-      <c r="Q58" s="309"/>
-      <c r="R58" s="309"/>
-      <c r="S58" s="309"/>
-      <c r="T58" s="310"/>
-      <c r="U58" s="311"/>
-      <c r="V58" s="312"/>
-      <c r="W58" s="313"/>
-      <c r="X58" s="311"/>
-      <c r="Y58" s="312"/>
-      <c r="Z58" s="317"/>
+      <c r="O58" s="301"/>
+      <c r="P58" s="301"/>
+      <c r="Q58" s="301"/>
+      <c r="R58" s="301"/>
+      <c r="S58" s="301"/>
+      <c r="T58" s="302"/>
+      <c r="U58" s="303"/>
+      <c r="V58" s="304"/>
+      <c r="W58" s="305"/>
+      <c r="X58" s="303"/>
+      <c r="Y58" s="304"/>
+      <c r="Z58" s="309"/>
       <c r="AA58" s="82"/>
       <c r="AB58" s="4" t="str">
         <f>PriceList!F56</f>
@@ -6113,36 +6105,36 @@
       <c r="AE58" s="84"/>
     </row>
     <row r="59" spans="1:31" s="71" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="308" t="s">
+      <c r="A59" s="300" t="s">
         <v>133</v>
       </c>
-      <c r="B59" s="309"/>
-      <c r="C59" s="309"/>
-      <c r="D59" s="309"/>
-      <c r="E59" s="309"/>
-      <c r="F59" s="309"/>
-      <c r="G59" s="310"/>
-      <c r="H59" s="311"/>
-      <c r="I59" s="312"/>
-      <c r="J59" s="313"/>
-      <c r="K59" s="322"/>
-      <c r="L59" s="323"/>
-      <c r="M59" s="324"/>
-      <c r="N59" s="318" t="s">
+      <c r="B59" s="301"/>
+      <c r="C59" s="301"/>
+      <c r="D59" s="301"/>
+      <c r="E59" s="301"/>
+      <c r="F59" s="301"/>
+      <c r="G59" s="302"/>
+      <c r="H59" s="303"/>
+      <c r="I59" s="304"/>
+      <c r="J59" s="305"/>
+      <c r="K59" s="314"/>
+      <c r="L59" s="315"/>
+      <c r="M59" s="316"/>
+      <c r="N59" s="310" t="s">
         <v>134</v>
       </c>
-      <c r="O59" s="309"/>
-      <c r="P59" s="309"/>
-      <c r="Q59" s="309"/>
-      <c r="R59" s="309"/>
-      <c r="S59" s="309"/>
-      <c r="T59" s="310"/>
-      <c r="U59" s="311"/>
-      <c r="V59" s="312"/>
-      <c r="W59" s="313"/>
-      <c r="X59" s="311"/>
-      <c r="Y59" s="312"/>
-      <c r="Z59" s="317"/>
+      <c r="O59" s="301"/>
+      <c r="P59" s="301"/>
+      <c r="Q59" s="301"/>
+      <c r="R59" s="301"/>
+      <c r="S59" s="301"/>
+      <c r="T59" s="302"/>
+      <c r="U59" s="303"/>
+      <c r="V59" s="304"/>
+      <c r="W59" s="305"/>
+      <c r="X59" s="303"/>
+      <c r="Y59" s="304"/>
+      <c r="Z59" s="309"/>
       <c r="AA59" s="82"/>
       <c r="AB59" s="4" t="str">
         <f>PriceList!F57</f>
@@ -6156,36 +6148,36 @@
       <c r="AE59" s="84"/>
     </row>
     <row r="60" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="337" t="s">
+      <c r="A60" s="329" t="s">
         <v>135</v>
       </c>
-      <c r="B60" s="338"/>
-      <c r="C60" s="338"/>
-      <c r="D60" s="338"/>
-      <c r="E60" s="338"/>
-      <c r="F60" s="338"/>
-      <c r="G60" s="339"/>
-      <c r="H60" s="340"/>
-      <c r="I60" s="341"/>
-      <c r="J60" s="342"/>
-      <c r="K60" s="325"/>
-      <c r="L60" s="326"/>
-      <c r="M60" s="327"/>
-      <c r="N60" s="343" t="s">
+      <c r="B60" s="330"/>
+      <c r="C60" s="330"/>
+      <c r="D60" s="330"/>
+      <c r="E60" s="330"/>
+      <c r="F60" s="330"/>
+      <c r="G60" s="331"/>
+      <c r="H60" s="332"/>
+      <c r="I60" s="333"/>
+      <c r="J60" s="334"/>
+      <c r="K60" s="317"/>
+      <c r="L60" s="318"/>
+      <c r="M60" s="319"/>
+      <c r="N60" s="335" t="s">
         <v>136</v>
       </c>
-      <c r="O60" s="344"/>
-      <c r="P60" s="344"/>
-      <c r="Q60" s="344"/>
-      <c r="R60" s="344"/>
-      <c r="S60" s="344"/>
-      <c r="T60" s="345"/>
-      <c r="U60" s="340"/>
-      <c r="V60" s="341"/>
-      <c r="W60" s="342"/>
-      <c r="X60" s="340"/>
-      <c r="Y60" s="341"/>
-      <c r="Z60" s="346"/>
+      <c r="O60" s="336"/>
+      <c r="P60" s="336"/>
+      <c r="Q60" s="336"/>
+      <c r="R60" s="336"/>
+      <c r="S60" s="336"/>
+      <c r="T60" s="337"/>
+      <c r="U60" s="332"/>
+      <c r="V60" s="333"/>
+      <c r="W60" s="334"/>
+      <c r="X60" s="332"/>
+      <c r="Y60" s="333"/>
+      <c r="Z60" s="338"/>
       <c r="AA60" s="82"/>
       <c r="AB60" s="4" t="str">
         <f>PriceList!F58</f>
@@ -6199,34 +6191,34 @@
       <c r="AE60" s="84"/>
     </row>
     <row r="61" spans="1:31" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="328"/>
-      <c r="B61" s="329"/>
-      <c r="C61" s="329"/>
-      <c r="D61" s="329"/>
-      <c r="E61" s="329"/>
-      <c r="F61" s="329"/>
-      <c r="G61" s="329"/>
-      <c r="H61" s="329"/>
-      <c r="I61" s="329"/>
-      <c r="J61" s="329"/>
-      <c r="K61" s="329"/>
-      <c r="L61" s="329"/>
-      <c r="M61" s="330"/>
-      <c r="N61" s="331" t="s">
+      <c r="A61" s="320"/>
+      <c r="B61" s="321"/>
+      <c r="C61" s="321"/>
+      <c r="D61" s="321"/>
+      <c r="E61" s="321"/>
+      <c r="F61" s="321"/>
+      <c r="G61" s="321"/>
+      <c r="H61" s="321"/>
+      <c r="I61" s="321"/>
+      <c r="J61" s="321"/>
+      <c r="K61" s="321"/>
+      <c r="L61" s="321"/>
+      <c r="M61" s="322"/>
+      <c r="N61" s="323" t="s">
         <v>137</v>
       </c>
-      <c r="O61" s="332"/>
-      <c r="P61" s="332"/>
-      <c r="Q61" s="332"/>
-      <c r="R61" s="332"/>
-      <c r="S61" s="332"/>
-      <c r="T61" s="333"/>
-      <c r="U61" s="334"/>
-      <c r="V61" s="335"/>
-      <c r="W61" s="335"/>
-      <c r="X61" s="335"/>
-      <c r="Y61" s="335"/>
-      <c r="Z61" s="336"/>
+      <c r="O61" s="324"/>
+      <c r="P61" s="324"/>
+      <c r="Q61" s="324"/>
+      <c r="R61" s="324"/>
+      <c r="S61" s="324"/>
+      <c r="T61" s="325"/>
+      <c r="U61" s="326"/>
+      <c r="V61" s="327"/>
+      <c r="W61" s="327"/>
+      <c r="X61" s="327"/>
+      <c r="Y61" s="327"/>
+      <c r="Z61" s="328"/>
       <c r="AA61" s="86"/>
       <c r="AB61" s="22"/>
       <c r="AC61" s="23"/>
@@ -6726,10 +6718,10 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B80" sqref="B80"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8086,7 +8078,7 @@
       </c>
       <c r="C50" s="61"/>
       <c r="D50" s="61">
-        <f>IF(AND(Agreement!S33&lt;&gt;0,Agreement!X33&lt;&gt;0),1,0)</f>
+        <f>IF(Agreement!X33&lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="E50" s="62">

</xml_diff>